<commit_message>
Ignorar carpeta de sesión en Git
</commit_message>
<xml_diff>
--- a/src/ProspectoBot.xlsx
+++ b/src/ProspectoBot.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="459">
   <si>
     <t>Fecha</t>
   </si>
@@ -1367,6 +1367,27 @@
   </si>
   <si>
     <t>11:00:21 a. m.</t>
+  </si>
+  <si>
+    <t>12:47:59 p. m.</t>
+  </si>
+  <si>
+    <t>2:17:57 p. m.</t>
+  </si>
+  <si>
+    <t>2:18:30 p. m.</t>
+  </si>
+  <si>
+    <t>miau y si deseo la inscripcion</t>
+  </si>
+  <si>
+    <t>2:18:49 p. m.</t>
+  </si>
+  <si>
+    <t>2:18:58 p. m.</t>
+  </si>
+  <si>
+    <t>Excel basico</t>
   </si>
 </sst>
 </file>
@@ -1743,7 +1764,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E275"/>
+  <dimension ref="A1:E280"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6421,6 +6442,91 @@
         <v>221</v>
       </c>
     </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>450</v>
+      </c>
+      <c r="B276" t="s">
+        <v>452</v>
+      </c>
+      <c r="C276" t="s">
+        <v>7</v>
+      </c>
+      <c r="D276" t="s">
+        <v>8</v>
+      </c>
+      <c r="E276" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>450</v>
+      </c>
+      <c r="B277" t="s">
+        <v>453</v>
+      </c>
+      <c r="C277" t="s">
+        <v>7</v>
+      </c>
+      <c r="D277" t="s">
+        <v>8</v>
+      </c>
+      <c r="E277" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>450</v>
+      </c>
+      <c r="B278" t="s">
+        <v>454</v>
+      </c>
+      <c r="C278" t="s">
+        <v>7</v>
+      </c>
+      <c r="D278" t="s">
+        <v>8</v>
+      </c>
+      <c r="E278" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>450</v>
+      </c>
+      <c r="B279" t="s">
+        <v>456</v>
+      </c>
+      <c r="C279" t="s">
+        <v>7</v>
+      </c>
+      <c r="D279" t="s">
+        <v>8</v>
+      </c>
+      <c r="E279" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>450</v>
+      </c>
+      <c r="B280" t="s">
+        <v>457</v>
+      </c>
+      <c r="C280" t="s">
+        <v>7</v>
+      </c>
+      <c r="D280" t="s">
+        <v>8</v>
+      </c>
+      <c r="E280" t="s">
+        <v>458</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>